<commit_message>
Adapt output directory style as maven and free.
</commit_message>
<xml_diff>
--- a/meta/program/BlancoValueObjectConstants.xlsx
+++ b/meta/program/BlancoValueObjectConstants.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10812"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tueda/data/webstorm/blanco/blancoValueObject/meta/program/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E46E8EFB-34C5-3746-BDEA-9E89B79AF6B4}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FF1EE27-7381-D440-820C-6DF857ED2107}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1580" yWindow="1300" windowWidth="20040" windowHeight="15020" tabRatio="575"/>
+    <workbookView xWindow="1580" yWindow="1300" windowWidth="20040" windowHeight="15020" tabRatio="575" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="constants" sheetId="1" r:id="rId1"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="52">
   <si>
     <t>定数定義書</t>
   </si>
@@ -163,13 +163,77 @@
   </si>
   <si>
     <t>"2.0.4"</t>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>TARGET_STYLE_BLANCO</t>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>java.lang.String</t>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>"blanco"</t>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>targetdirに設定される文字列</t>
+    <rPh sb="10" eb="12">
+      <t xml:space="preserve">セッテイ </t>
+    </rPh>
+    <rPh sb="15" eb="18">
+      <t xml:space="preserve">モジレツ </t>
+    </rPh>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>TARGET_STYLE_MAVEN</t>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>TARGET_STYLE_FREE</t>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>"maven"</t>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>"free"</t>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>"main"</t>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>生成したソースコードを保管するディレクトリのsuffix</t>
+    <rPh sb="0" eb="2">
+      <t xml:space="preserve">セイセイ </t>
+    </rPh>
+    <rPh sb="11" eb="13">
+      <t xml:space="preserve">ホカンスル </t>
+    </rPh>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>TARGET_DIR_SUFFIX_BLANCO</t>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>TARGET_DIR_SUFFIX_MAVEN</t>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>"main/java"</t>
     <phoneticPr fontId="4"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="5">
     <font>
       <sz val="11"/>
@@ -1071,14 +1135,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:H33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+      <selection activeCell="E29" sqref="E29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14"/>
@@ -1347,51 +1411,101 @@
       <c r="H23"/>
     </row>
     <row r="24" spans="1:8">
-      <c r="A24" s="24"/>
-      <c r="B24" s="25"/>
-      <c r="C24" s="26"/>
-      <c r="D24" s="26"/>
-      <c r="E24" s="26"/>
+      <c r="A24" s="24">
+        <v>5</v>
+      </c>
+      <c r="B24" s="25" t="s">
+        <v>39</v>
+      </c>
+      <c r="C24" s="26" t="s">
+        <v>40</v>
+      </c>
+      <c r="D24" s="26" t="s">
+        <v>41</v>
+      </c>
+      <c r="E24" s="26" t="s">
+        <v>42</v>
+      </c>
       <c r="F24" s="30"/>
       <c r="G24"/>
       <c r="H24"/>
     </row>
     <row r="25" spans="1:8">
-      <c r="A25" s="24"/>
-      <c r="B25" s="25"/>
-      <c r="C25" s="26"/>
-      <c r="D25" s="26"/>
-      <c r="E25" s="26"/>
+      <c r="A25" s="24">
+        <v>6</v>
+      </c>
+      <c r="B25" s="25" t="s">
+        <v>43</v>
+      </c>
+      <c r="C25" s="26" t="s">
+        <v>40</v>
+      </c>
+      <c r="D25" s="26" t="s">
+        <v>45</v>
+      </c>
+      <c r="E25" s="26" t="s">
+        <v>42</v>
+      </c>
       <c r="F25" s="30"/>
       <c r="G25"/>
       <c r="H25"/>
     </row>
     <row r="26" spans="1:8">
-      <c r="A26" s="24"/>
-      <c r="B26" s="25"/>
-      <c r="C26" s="26"/>
-      <c r="D26" s="26"/>
-      <c r="E26" s="26"/>
+      <c r="A26" s="24">
+        <v>7</v>
+      </c>
+      <c r="B26" s="25" t="s">
+        <v>44</v>
+      </c>
+      <c r="C26" s="26" t="s">
+        <v>40</v>
+      </c>
+      <c r="D26" s="26" t="s">
+        <v>46</v>
+      </c>
+      <c r="E26" s="26" t="s">
+        <v>42</v>
+      </c>
       <c r="F26" s="30"/>
       <c r="G26"/>
       <c r="H26"/>
     </row>
     <row r="27" spans="1:8">
-      <c r="A27" s="24"/>
-      <c r="B27" s="25"/>
-      <c r="C27" s="26"/>
-      <c r="D27" s="26"/>
-      <c r="E27" s="26"/>
+      <c r="A27" s="24">
+        <v>8</v>
+      </c>
+      <c r="B27" s="25" t="s">
+        <v>49</v>
+      </c>
+      <c r="C27" s="26" t="s">
+        <v>40</v>
+      </c>
+      <c r="D27" s="26" t="s">
+        <v>47</v>
+      </c>
+      <c r="E27" s="26" t="s">
+        <v>48</v>
+      </c>
       <c r="F27" s="30"/>
       <c r="G27"/>
       <c r="H27"/>
     </row>
     <row r="28" spans="1:8">
-      <c r="A28" s="31"/>
-      <c r="B28" s="25"/>
-      <c r="C28" s="32"/>
-      <c r="D28" s="32"/>
-      <c r="E28" s="32"/>
+      <c r="A28" s="24">
+        <v>8</v>
+      </c>
+      <c r="B28" s="25" t="s">
+        <v>50</v>
+      </c>
+      <c r="C28" s="26" t="s">
+        <v>40</v>
+      </c>
+      <c r="D28" s="26" t="s">
+        <v>51</v>
+      </c>
+      <c r="E28" s="26" t="s">
+        <v>48</v>
+      </c>
       <c r="F28" s="33"/>
       <c r="G28"/>
       <c r="H28"/>
@@ -1445,19 +1559,19 @@
   </mergeCells>
   <phoneticPr fontId="4"/>
   <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="D47">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="D47" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>型</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="C12">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="C12" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>adjustConstValue</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="C11">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="C11" xr:uid="{00000000-0002-0000-0000-000002000000}">
       <formula1>isAbstract</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="C10">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="C10" xr:uid="{00000000-0002-0000-0000-000003000000}">
       <formula1>accessScope</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -1471,7 +1585,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:J6"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>